<commit_message>
Created event database template and filler data in excel files
Both .xslx and .csv files
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF4C82C-999E-6D41-9777-F65581ECF388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B32DC3-8CFA-2249-B6F1-C6E65A0F8821}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{041EF0F1-DB8B-D74B-AF2D-7B6D7E9ECA55}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,35 +31,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>event_name</t>
   </si>
   <si>
+    <t>organiser_id</t>
+  </si>
+  <si>
     <t>start_date</t>
   </si>
   <si>
-    <t>organiser_id</t>
-  </si>
-  <si>
     <t>end_date</t>
   </si>
   <si>
     <t>address</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
-    <t>dateTime</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -72,26 +63,137 @@
     <t>available_tickets</t>
   </si>
   <si>
-    <t>tinytext</t>
-  </si>
-  <si>
-    <t>double(6, 2)</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>smallInt</t>
+    <t>CodeMaster Fyre</t>
+  </si>
+  <si>
+    <t>Laneway Festival</t>
+  </si>
+  <si>
+    <t>Andy Warhol Exhibition</t>
+  </si>
+  <si>
+    <t>Optus Stadium</t>
+  </si>
+  <si>
+    <t>Northbridge Piazza</t>
+  </si>
+  <si>
+    <t>Family Movie Night - Shrek</t>
+  </si>
+  <si>
+    <t>Perth Wildcats Vs. Sydney Kings</t>
+  </si>
+  <si>
+    <t>A-Team Vs. AAA-Team</t>
+  </si>
+  <si>
+    <t>Fiyoari, Maldives</t>
+  </si>
+  <si>
+    <t>56 Moonwalk Lane, Boogie Town WA</t>
+  </si>
+  <si>
+    <t>Perth Arena</t>
+  </si>
+  <si>
+    <t>Elizabeth Key</t>
+  </si>
+  <si>
+    <t>Perth Museum</t>
+  </si>
+  <si>
+    <t>Fremantle Esplanade</t>
+  </si>
+  <si>
+    <t>10$ Cocktail Thursdays</t>
+  </si>
+  <si>
+    <t>Hula Bula Bar</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Fringe Festival</t>
+  </si>
+  <si>
+    <t>CodeMaster Institute</t>
+  </si>
+  <si>
+    <t>West Coast Eagles Vs. Fremantle Dockers</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed malesuada, sapien at varius interdum, enim enim mattis nisi, non faucibus erat tortor et felis. In ac condimentum libero, id viverra nisi. Vivamus ullamcorper placerat mi, quis porta magna vestibulum sed. Nunc vitae lorem eget magna porttitor tempor. Aenean commodo elit sit amet justo fringilla, at placerat magna laoreet. Fusce ipsum metus, tristique nec commodo et, posuere a mi. Sed dapibus libero ut nunc pellentesque feugiat. Quisque tincidunt blandit nisi.
+Mauris accumsan hendrerit sem sed bibendum. Maecenas tempus, mi et venenatis commodo, diam ex auctor metus, quis congue eros ligula vitae eros. Nunc vitae ultricies sem. Curabitur blandit luctus sapien, at efficitur urna. Ut purus leo, interdum eget nunc id, molestie dignissim nibh. Donec condimentum metus non dui pretium varius. Curabitur tempus nunc sed fringilla sodales. Vivamus commodo consectetur ipsum et malesuada. Nulla facilisi. Praesent sed tortor at ex aliquet feugiat. Integer ornare euismod lorem. Curabitur finibus lectus mollis mi placerat, ac tincidunt massa laoreet. Nunc quam diam, mollis scelerisque dui et, bibendum blandit massa. Fusce eget quam pellentesque, ornare felis id, fermentum felis. Pellentesque eget malesuada eros. Curabitur tincidunt enim ac varius sodales.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2019-04-19 10:00:00</t>
+  </si>
+  <si>
+    <t>2019-05-24 17:00:00</t>
+  </si>
+  <si>
+    <t>2019-04-19 20:00:00</t>
+  </si>
+  <si>
+    <t>2019-04-20 01:00:00</t>
+  </si>
+  <si>
+    <t>So Fresh Concert Autumn 2004</t>
+  </si>
+  <si>
+    <t>andy.jpeg</t>
+  </si>
+  <si>
+    <t>ateam.jpg</t>
+  </si>
+  <si>
+    <t>codemaster.jpg</t>
+  </si>
+  <si>
+    <t>fringe.jpg</t>
+  </si>
+  <si>
+    <t>sofresh.jpg</t>
+  </si>
+  <si>
+    <t>shrek.jpg</t>
+  </si>
+  <si>
+    <t>westcoastfremantle.jpg</t>
+  </si>
+  <si>
+    <t>wildcatssydneykings.jpg</t>
+  </si>
+  <si>
+    <t>hulabula.jpg</t>
+  </si>
+  <si>
+    <t>laneway.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,8 +219,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,77 +541,376 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA8E7AC-456C-A642-8935-CEEF2F09E7C2}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00D733E-37AC-3A4A-9EF4-7A258438F26A}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>69</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B11" t="s">
         <v>16</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>37</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel database templates
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B32DC3-8CFA-2249-B6F1-C6E65A0F8821}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F21993-B1BA-E84C-9605-27A0DEB6EBAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
@@ -142,9 +142,6 @@
     <t>2019-04-20 01:00:00</t>
   </si>
   <si>
-    <t>So Fresh Concert Autumn 2004</t>
-  </si>
-  <si>
     <t>andy.jpeg</t>
   </si>
   <si>
@@ -166,13 +163,16 @@
     <t>westcoastfremantle.jpg</t>
   </si>
   <si>
-    <t>wildcatssydneykings.jpg</t>
-  </si>
-  <si>
     <t>hulabula.jpg</t>
   </si>
   <si>
     <t>laneway.jpg</t>
+  </si>
+  <si>
+    <t>So Fresh Concert</t>
+  </si>
+  <si>
+    <t>wildcatskings.jpg</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -651,7 +651,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3">
         <v>300</v>
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4">
         <v>50</v>
@@ -715,7 +715,7 @@
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
         <v>31</v>
@@ -747,7 +747,7 @@
         <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6">
         <v>8000</v>
@@ -779,7 +779,7 @@
         <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
         <v>31</v>
@@ -790,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -811,7 +811,7 @@
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8">
         <v>10000</v>
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9">
         <v>50</v>
@@ -875,7 +875,7 @@
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10">
         <v>65000</v>
@@ -907,7 +907,7 @@
         <v>30</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J11">
         <v>20000</v>

</xml_diff>

<commit_message>
Changed config file and database excel templates
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F21993-B1BA-E84C-9605-27A0DEB6EBAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A57C1F5-0945-DD4E-8D38-F179A1DFFBB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
@@ -33,36 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>event_name</t>
-  </si>
-  <si>
-    <t>organiser_id</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>available_tickets</t>
-  </si>
-  <si>
     <t>CodeMaster Fyre</t>
   </si>
   <si>
@@ -173,6 +143,36 @@
   </si>
   <si>
     <t>wildcatskings.jpg</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>organiser_id</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>available_tickets</t>
+  </si>
+  <si>
+    <t>identification</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -561,36 +561,36 @@
     <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -598,28 +598,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -630,28 +630,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>10000</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>300</v>
@@ -662,28 +662,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="J4">
         <v>50</v>
@@ -694,31 +694,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -726,28 +726,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="J6">
         <v>8000</v>
@@ -758,31 +758,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
         <v>19.989999999999998</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -790,28 +790,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2">
         <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
         <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
       </c>
       <c r="J8">
         <v>10000</v>
@@ -822,28 +822,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="J9">
         <v>50</v>
@@ -854,28 +854,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>69</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="J10">
         <v>65000</v>
@@ -886,28 +886,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>37</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J11">
         <v>20000</v>

</xml_diff>

<commit_message>
Edit the excel database templates
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A57C1F5-0945-DD4E-8D38-F179A1DFFBB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32176D68-E42D-AE4A-84C7-D7D4D9CFACFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
@@ -97,9 +97,6 @@
 Mauris accumsan hendrerit sem sed bibendum. Maecenas tempus, mi et venenatis commodo, diam ex auctor metus, quis congue eros ligula vitae eros. Nunc vitae ultricies sem. Curabitur blandit luctus sapien, at efficitur urna. Ut purus leo, interdum eget nunc id, molestie dignissim nibh. Donec condimentum metus non dui pretium varius. Curabitur tempus nunc sed fringilla sodales. Vivamus commodo consectetur ipsum et malesuada. Nulla facilisi. Praesent sed tortor at ex aliquet feugiat. Integer ornare euismod lorem. Curabitur finibus lectus mollis mi placerat, ac tincidunt massa laoreet. Nunc quam diam, mollis scelerisque dui et, bibendum blandit massa. Fusce eget quam pellentesque, ornare felis id, fermentum felis. Pellentesque eget malesuada eros. Curabitur tincidunt enim ac varius sodales.</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2019-04-19 10:00:00</t>
   </si>
   <si>
@@ -173,16 +170,15 @@
   </si>
   <si>
     <t>identification</t>
+  </si>
+  <si>
+    <t>unlimited</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -221,13 +217,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +541,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -555,7 +551,7 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -563,34 +559,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -603,23 +599,23 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -635,23 +631,23 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>10000</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>300</v>
@@ -667,23 +663,23 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>45</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>50</v>
@@ -699,26 +695,26 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -731,23 +727,23 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>8000</v>
@@ -763,26 +759,26 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>19.989999999999998</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -790,28 +786,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>10</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>10000</v>
@@ -827,23 +823,23 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>5</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9">
         <v>50</v>
@@ -859,23 +855,23 @@
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>69</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J10">
         <v>65000</v>
@@ -891,23 +887,23 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>37</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11">
         <v>20000</v>

</xml_diff>

<commit_message>
Added categories column and categories to databases
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32176D68-E42D-AE4A-84C7-D7D4D9CFACFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF9A839-F6FF-3F4F-9189-754C675CBF3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>CodeMaster Fyre</t>
   </si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>unlimited</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>food and drink</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>art</t>
+  </si>
+  <si>
+    <t>family</t>
   </si>
 </sst>
 </file>
@@ -538,26 +559,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00D733E-37AC-3A4A-9EF4-7A258438F26A}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -565,347 +587,380 @@
         <v>36</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>10000</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>45</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>26</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>33</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>19.989999999999998</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>29</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>5</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>30</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>69</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>31</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>65000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>37</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>35</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>20000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated database with capitalised category values
</commit_message>
<xml_diff>
--- a/databases/events/events.xlsx
+++ b/databases/events/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminnewton/Dropbox/Benjamin Peter Newton/Websites/A-Team/databases/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF9A839-F6FF-3F4F-9189-754C675CBF3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5C93FD-3945-2B4E-BF48-76A48DC2D695}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F15F53ED-B823-9242-9BF7-D11B1FA70681}"/>
   </bookViews>
@@ -178,22 +178,22 @@
     <t>category</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>sport</t>
-  </si>
-  <si>
-    <t>food and drink</t>
-  </si>
-  <si>
-    <t>music</t>
-  </si>
-  <si>
-    <t>art</t>
-  </si>
-  <si>
-    <t>family</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Food and Drink</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Family</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -832,7 +832,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>7</v>

</xml_diff>